<commit_message>
2021-07-02 JCS : retirer lien evento
</commit_message>
<xml_diff>
--- a/FulUserOverdueNoticeLetter/FulUserOverdueNoticeLetter.xlsx
+++ b/FulUserOverdueNoticeLetter/FulUserOverdueNoticeLetter.xlsx
@@ -361,12 +361,12 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t/>
+          <t>EMPTY_STRING</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>En raison du contexte sanitaire, la prise de rendez-vous est obligatoire. Vous pouvez sélectionner un créneau en suivant ce lien : https://evento.renater.fr/survey/acces-au-ged-hors-les-murs-pendant-le-confinement-o0zy4wzf</t>
+          <t>EMPTY_STRING</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -375,7 +375,7 @@
         </is>
       </c>
       <c r="F9" s="1" t="n">
-        <v>44201.0</v>
+        <v>44379.0</v>
       </c>
     </row>
     <row r="10">

</xml_diff>